<commit_message>
Editing the timesheet from week 10 till week 13
</commit_message>
<xml_diff>
--- a/Timesheet_a1760776_Neha Wali.xlsx
+++ b/Timesheet_a1760776_Neha Wali.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20358"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{176AFAB2-578F-46D4-B3A0-C29BF2A56704}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2814D481-ADE2-45D6-B95E-821BDA211CE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="8" xr2:uid="{C15D630B-6CCD-4C89-A3BE-DC5AA8491586}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="12" xr2:uid="{C15D630B-6CCD-4C89-A3BE-DC5AA8491586}"/>
   </bookViews>
   <sheets>
     <sheet name="week 2" sheetId="2" r:id="rId1"/>
@@ -22,18 +22,30 @@
     <sheet name="week 7" sheetId="7" r:id="rId7"/>
     <sheet name="week 8" sheetId="8" r:id="rId8"/>
     <sheet name="week 9" sheetId="9" r:id="rId9"/>
+    <sheet name="week 10" sheetId="10" r:id="rId10"/>
+    <sheet name="week 11" sheetId="11" r:id="rId11"/>
+    <sheet name="week 12" sheetId="12" r:id="rId12"/>
+    <sheet name="week 13" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="150">
   <si>
     <t>Day</t>
   </si>
@@ -380,19 +392,115 @@
     <t>Doing unit testing and integration testing on parsons puzzle funcion. Moreover, while testing finding if finding some issues, reporting it to the developer.(for example: errors or buttons not working).</t>
   </si>
   <si>
-    <t>Brainstorming session with the team about design and how to conclude the research we hav edone all along.</t>
-  </si>
-  <si>
     <t>Editing the testing report and researching about the design of creation of parsons puzzle and evaluating different types and their significance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week : 12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week : 11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week : 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week : 13 </t>
+  </si>
+  <si>
+    <t>Drafting the final design document by structuring thoughts and creating the student and instructure interface GUI</t>
+  </si>
+  <si>
+    <t>18.05.2020</t>
+  </si>
+  <si>
+    <t>20.05.2020</t>
+  </si>
+  <si>
+    <t>21.05.2020</t>
+  </si>
+  <si>
+    <t>22.05.2020</t>
+  </si>
+  <si>
+    <t>23.05.2020</t>
+  </si>
+  <si>
+    <t>Updating the final design document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing the feedback part of the the Drag and Drop function committed to GitHub </t>
+  </si>
+  <si>
+    <t>Discussion of final design document, final milestone and reflecting on previous communication gap, to not commit it into final milestone</t>
+  </si>
+  <si>
+    <t>24.05.2020</t>
+  </si>
+  <si>
+    <t>27.05.2020</t>
+  </si>
+  <si>
+    <t>Structuring the poster layout, and starting to finalise the heading and add the content in parts of Introduction and Tools.</t>
+  </si>
+  <si>
+    <t>28.05.2020</t>
+  </si>
+  <si>
+    <t>Meeting with the supervisor. Report the progress. Discuss the goal for the final milestone: feedback function and fill in the blanks.</t>
+  </si>
+  <si>
+    <t>Brainstorming session with the team about design and how to conclude the research we have done all along.</t>
+  </si>
+  <si>
+    <t>Creating the GUI for the design document and specifying the content to be added for future extension of design</t>
+  </si>
+  <si>
+    <t>Adding the content into poster, and summarising the universal design key concepts</t>
+  </si>
+  <si>
+    <t>Editing the meeting minutes from week 7 till week 12, and finalising the poster by doing grammatical checks and combining the parts together</t>
+  </si>
+  <si>
+    <t>05.06.2020</t>
+  </si>
+  <si>
+    <t>06.06.2020</t>
+  </si>
+  <si>
+    <t>07.06.2020</t>
+  </si>
+  <si>
+    <t>Finalising the design document, and combining the GUI with content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding the predefined syntax rule of the H5P customised function and analysing the integration implemented in second version, testing the version. </t>
+  </si>
+  <si>
+    <t>08.06.2020</t>
+  </si>
+  <si>
+    <t>Updating the poster and the final design document by taking feedback from the supervisor</t>
+  </si>
+  <si>
+    <t>19.06.2020</t>
+  </si>
+  <si>
+    <t>Meeting with the supervisor, showing the demo video and taking suggestion for structuring demo</t>
+  </si>
+  <si>
+    <t>29.05.2020</t>
+  </si>
+  <si>
+    <t>Going through poster examples and collecting data for poster, getting idea about demo and final report</t>
+  </si>
+  <si>
+    <t>Assessing the implementation of the design done by technical team and thinking how to extend the project design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="hh:mm"/>
-  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -578,7 +686,7 @@
     <xf numFmtId="20" fontId="4" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -602,80 +710,80 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -760,37 +868,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -875,37 +983,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -990,37 +1098,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1105,37 +1213,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1220,37 +1328,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1335,37 +1443,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1450,37 +1558,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1565,37 +1673,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -2041,13 +2149,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="1" max="2" width="12.6328125" customWidth="1"/>
+    <col min="6" max="6" width="100.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2057,7 +2165,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2073,7 +2181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2093,7 +2201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -2113,7 +2221,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -2133,7 +2241,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -2153,7 +2261,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2164,17 +2272,613 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1935E846-ED74-4E62-9E65-750E1CE1D83B}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="100.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E6" s="3">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6">
+        <f>SUBTOTAL(109,E6:E11)</f>
+        <v>23</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AF2CCF-03B0-4010-9C07-03185F1A3114}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="100.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E6" s="3">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6">
+        <f>SUBTOTAL(109,E6:E9)</f>
+        <v>25</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA9CC2F-7A9A-4A67-B7CD-13F59E8EAD1D}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="100.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E6" s="3">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6">
+        <f>SUBTOTAL(109,E6:E8)</f>
+        <v>25</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6ECA9F9-B1F4-44FB-8CDA-C810616503BC}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="100.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E6" s="3">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6">
+        <f>SUBTOTAL(109,E6:E7)</f>
+        <v>9</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2186,13 +2890,13 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="1" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="100.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2204,7 +2908,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2221,7 +2925,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2241,7 +2945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -2261,7 +2965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -2281,7 +2985,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -2301,7 +3005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -2321,7 +3025,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -2341,7 +3045,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -2361,7 +3065,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -2381,7 +3085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -2401,7 +3105,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
@@ -2421,7 +3125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -2449,12 +3153,12 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="6" max="6" width="100.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2464,7 +3168,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2480,7 +3184,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2500,7 +3204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -2520,7 +3224,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2540,7 +3244,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -2560,7 +3264,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -2580,7 +3284,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -2600,7 +3304,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -2620,7 +3324,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2631,9 +3335,9 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2650,14 +3354,14 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2667,7 +3371,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2683,7 +3387,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2703,7 +3407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -2723,7 +3427,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -2743,7 +3447,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -2763,7 +3467,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -2783,7 +3487,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -2803,7 +3507,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -2823,7 +3527,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2834,9 +3538,9 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2853,12 +3557,12 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="6" max="6" width="100.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2868,7 +3572,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2884,7 +3588,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2904,7 +3608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -2924,7 +3628,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -2944,7 +3648,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -2964,7 +3668,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -2984,7 +3688,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -3004,7 +3708,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -3024,7 +3728,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -3044,7 +3748,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -3055,8 +3759,8 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>73</v>
       </c>
@@ -3077,13 +3781,13 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="100.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3093,7 +3797,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3109,7 +3813,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -3129,7 +3833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -3149,7 +3853,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>86</v>
       </c>
@@ -3169,7 +3873,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -3189,7 +3893,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -3209,7 +3913,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -3236,13 +3940,13 @@
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="150.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="150.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3252,7 +3956,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3268,7 +3972,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -3288,7 +3992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -3308,7 +4012,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -3328,7 +4032,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -3348,7 +4052,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -3368,7 +4072,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -3388,7 +4092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -3408,7 +4112,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -3435,12 +4139,12 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="150.77734375" customWidth="1"/>
+    <col min="6" max="6" width="150.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3450,7 +4154,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3466,7 +4170,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -3486,7 +4190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -3506,7 +4210,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -3526,7 +4230,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -3546,7 +4250,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -3566,7 +4270,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -3586,7 +4290,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -3609,16 +4313,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E05878C-74C7-49DA-885D-D3B84DD5D977}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="150.77734375" customWidth="1"/>
+    <col min="6" max="6" width="150.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3628,7 +4332,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3644,7 +4348,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -3667,7 +4371,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -3690,7 +4394,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -3711,7 +4415,7 @@
       </c>
       <c r="G7" s="13"/>
     </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -3728,11 +4432,11 @@
         <v>3</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -3749,11 +4453,11 @@
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>

</xml_diff>

<commit_message>
Editing the date which I entered wrongly for week 13. 19.06.2020 instead of 09.06.2020.
</commit_message>
<xml_diff>
--- a/Timesheet_a1760776_Neha Wali.xlsx
+++ b/Timesheet_a1760776_Neha Wali.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2814D481-ADE2-45D6-B95E-821BDA211CE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8138180-D35D-4B3F-AEAA-55B3E5022B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="12" xr2:uid="{C15D630B-6CCD-4C89-A3BE-DC5AA8491586}"/>
   </bookViews>
@@ -482,9 +482,6 @@
     <t>Updating the poster and the final design document by taking feedback from the supervisor</t>
   </si>
   <si>
-    <t>19.06.2020</t>
-  </si>
-  <si>
     <t>Meeting with the supervisor, showing the demo video and taking suggestion for structuring demo</t>
   </si>
   <si>
@@ -495,6 +492,9 @@
   </si>
   <si>
     <t>Assessing the implementation of the design done by technical team and thinking how to extend the project design</t>
+  </si>
+  <si>
+    <t>09.06.2020</t>
   </si>
 </sst>
 </file>
@@ -2458,7 +2458,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
@@ -2593,7 +2593,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
@@ -2601,7 +2601,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" s="4">
         <v>0.5</v>
@@ -2772,7 +2772,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
@@ -2851,7 +2851,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C7" s="4">
         <v>0.625</v>
@@ -2863,7 +2863,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updating timesheet till week 13
</commit_message>
<xml_diff>
--- a/Timesheet_a1760776_Neha Wali.xlsx
+++ b/Timesheet_a1760776_Neha Wali.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20361"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04EAF94-BD1C-4505-9A97-0A68C45BF39D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DA9B88-39AE-4BE3-B908-8AEDDB7A52BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="11" xr2:uid="{C15D630B-6CCD-4C89-A3BE-DC5AA8491586}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="3" activeTab="12" xr2:uid="{C15D630B-6CCD-4C89-A3BE-DC5AA8491586}"/>
   </bookViews>
   <sheets>
     <sheet name="week 2" sheetId="2" r:id="rId1"/>
@@ -26,26 +26,19 @@
     <sheet name="week 11" sheetId="11" r:id="rId11"/>
     <sheet name="week 12" sheetId="12" r:id="rId12"/>
     <sheet name="week 13" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="167">
   <si>
     <t>Day</t>
   </si>
@@ -510,6 +503,42 @@
   </si>
   <si>
     <t>Discussion about demo and poster, and updates about progress for final milestone</t>
+  </si>
+  <si>
+    <t>Discuss the process and details of final presentation</t>
+  </si>
+  <si>
+    <t>Final Presentation Preparation: write speech and modify demo video</t>
+  </si>
+  <si>
+    <t>Rehearse with Supervisor</t>
+  </si>
+  <si>
+    <t>Practice demo</t>
+  </si>
+  <si>
+    <t>Final Presentation</t>
+  </si>
+  <si>
+    <t>Write final report</t>
+  </si>
+  <si>
+    <t>Create the initial vesion of demo ppt</t>
+  </si>
+  <si>
+    <t>Preapring the structure for speaking in demo and preparing the ppt for demo</t>
+  </si>
+  <si>
+    <t>14.06.2020</t>
+  </si>
+  <si>
+    <t>10.06.2020</t>
+  </si>
+  <si>
+    <t>11.06.2020</t>
+  </si>
+  <si>
+    <t>13.06.2020</t>
   </si>
 </sst>
 </file>
@@ -725,80 +754,80 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -883,37 +912,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -998,37 +1027,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1113,37 +1142,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1228,37 +1257,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1343,37 +1372,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1458,37 +1487,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1573,37 +1602,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -1688,37 +1717,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF3F3F3F"/>
-        <name val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -2164,13 +2193,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="100.6328125" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2180,7 +2209,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2196,7 +2225,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2216,7 +2245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -2236,7 +2265,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -2256,7 +2285,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -2276,7 +2305,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2287,12 +2316,12 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2309,12 +2338,12 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="100.81640625" customWidth="1"/>
+    <col min="6" max="6" width="100.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2324,7 +2353,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2340,7 +2369,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2360,7 +2389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -2380,7 +2409,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -2400,7 +2429,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -2420,7 +2449,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
@@ -2436,7 +2465,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -2456,7 +2485,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -2476,7 +2505,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2500,12 +2529,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="100.81640625" customWidth="1"/>
+    <col min="6" max="6" width="100.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2515,7 +2544,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2531,7 +2560,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2551,7 +2580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -2571,7 +2600,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2591,7 +2620,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -2611,7 +2640,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -2631,7 +2660,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -2651,7 +2680,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2671,16 +2700,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA9CC2F-7A9A-4A67-B7CD-13F59E8EAD1D}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="100.81640625" customWidth="1"/>
+    <col min="6" max="6" width="100.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2690,7 +2719,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2706,7 +2735,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2726,7 +2755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -2746,7 +2775,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -2766,7 +2795,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -2786,7 +2815,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
@@ -2806,7 +2835,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2824,18 +2853,19 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6ECA9F9-B1F4-44FB-8CDA-C810616503BC}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="100.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="100.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2845,7 +2875,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2861,7 +2891,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2881,7 +2911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -2901,7 +2931,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -2921,18 +2951,190 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6">
-        <f>SUBTOTAL(109,E6:E7)</f>
-        <v>9</v>
-      </c>
-      <c r="F8" s="6"/>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E15" s="3">
+        <v>13</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="3">
+        <v>15</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="6">
+        <f>SUBTOTAL(109,E6:E16)</f>
+        <v>54</v>
+      </c>
+      <c r="F17" s="6"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED064E8C-02C9-4591-A24D-A89998092AB0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2945,13 +3147,13 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="10.6328125" customWidth="1"/>
-    <col min="6" max="6" width="100.6328125" customWidth="1"/>
+    <col min="1" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2963,7 +3165,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2980,7 +3182,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -3000,7 +3202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -3020,7 +3222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -3040,7 +3242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -3060,7 +3262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -3080,7 +3282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -3100,7 +3302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -3120,7 +3322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -3140,7 +3342,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -3160,7 +3362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
@@ -3180,7 +3382,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -3208,12 +3410,12 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="100.6328125" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3223,7 +3425,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3239,7 +3441,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -3259,7 +3461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -3279,7 +3481,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -3299,7 +3501,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -3319,7 +3521,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -3339,7 +3541,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -3359,7 +3561,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -3379,7 +3581,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -3390,9 +3592,9 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3409,14 +3611,14 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="100.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3426,7 +3628,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3442,7 +3644,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -3462,7 +3664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -3482,7 +3684,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -3502,7 +3704,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -3522,7 +3724,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -3542,7 +3744,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -3562,7 +3764,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -3582,7 +3784,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -3593,9 +3795,9 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3612,12 +3814,12 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="100.6328125" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3627,7 +3829,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3643,7 +3845,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -3663,7 +3865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -3683,7 +3885,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -3703,7 +3905,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -3723,7 +3925,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -3743,7 +3945,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -3763,7 +3965,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -3783,7 +3985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -3803,7 +4005,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -3814,8 +4016,8 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>73</v>
       </c>
@@ -3836,13 +4038,13 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.6328125" customWidth="1"/>
-    <col min="6" max="6" width="100.6328125" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3852,7 +4054,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3868,7 +4070,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -3888,7 +4090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -3908,7 +4110,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>86</v>
       </c>
@@ -3928,7 +4130,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -3948,7 +4150,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -3968,7 +4170,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -3995,13 +4197,13 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.6328125" customWidth="1"/>
-    <col min="6" max="6" width="150.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="150.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -4011,7 +4213,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4027,7 +4229,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -4047,7 +4249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -4067,7 +4269,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -4087,7 +4289,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -4107,7 +4309,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -4127,7 +4329,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -4147,7 +4349,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -4167,7 +4369,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -4194,12 +4396,12 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="150.81640625" customWidth="1"/>
+    <col min="6" max="6" width="150.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -4209,7 +4411,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4225,7 +4427,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -4245,7 +4447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -4265,7 +4467,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -4285,7 +4487,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -4305,7 +4507,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -4325,7 +4527,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -4345,7 +4547,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -4372,12 +4574,12 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="150.81640625" customWidth="1"/>
+    <col min="6" max="6" width="150.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -4387,7 +4589,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4403,7 +4605,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -4426,7 +4628,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -4449,7 +4651,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -4470,7 +4672,7 @@
       </c>
       <c r="G7" s="13"/>
     </row>
-    <row r="8" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -4491,7 +4693,7 @@
       </c>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -4512,7 +4714,7 @@
       </c>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -4533,7 +4735,7 @@
       </c>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:7" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>

</xml_diff>